<commit_message>
Datatables delete from Diet_Plan.html
</commit_message>
<xml_diff>
--- a/backdata/stepid_list.xlsx
+++ b/backdata/stepid_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shunichinakada/Documents/webApp/ifna_pwa02/backdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F0E960-F753-8243-B37A-5BC6E2DDD9CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC54494-8CDC-D24C-B213-9B23B4D32A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="28300" windowHeight="17040" xr2:uid="{1F61A881-959B-2341-86FC-3A24FAE8EC45}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>stepid</t>
     <phoneticPr fontId="1"/>
@@ -120,6 +120,10 @@
   </si>
   <si>
     <t>output4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>location_create</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -144,12 +148,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -166,8 +182,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -484,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F47753-A97D-9B44-B3D8-131FCE61482E}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -586,7 +608,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>400</v>
       </c>
       <c r="B7" t="s">
@@ -600,7 +622,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>500</v>
       </c>
       <c r="B8" t="s">
@@ -628,7 +650,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>700</v>
       </c>
       <c r="B10" t="s">
@@ -642,7 +664,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>800</v>
       </c>
       <c r="B11" t="s">
@@ -697,7 +719,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>805</v>
       </c>
       <c r="B16" t="s">
@@ -708,7 +730,7 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>701</v>
       </c>
       <c r="B17" t="s">
@@ -729,7 +751,7 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -741,17 +763,6 @@
       </c>
       <c r="C19" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>814</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>